<commit_message>
SP Update: Refactored Expressions Evaluator using SQLA
</commit_message>
<xml_diff>
--- a/Sprint03_Data_Operation/_jonhonda_dat/special_prj/Input_Files/BMP Lego Piece.xlsx
+++ b/Sprint03_Data_Operation/_jonhonda_dat/special_prj/Input_Files/BMP Lego Piece.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JonHonda\OneDrive\Projects\Big Data School\BigDataAnalyst_ProjectDocumentation\Sprint03_Data_Operation\_jonhonda_dat\special_prj\Input_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Projects\Big Data School\BigDataAnalyst_ProjectDocumentation\Sprint03_Data_Operation\_jonhonda_dat\special_prj\Input_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="D3CBFCB539476F3AB5D5C1344C094AEA2BA55794" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{DB4262D7-AC80-4C46-85F3-2A5DD404793F}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="D3CBFCB539476F3AB5D5C1344C094AEA2BA55794" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{DB4262D7-AC80-4C46-85F3-2A5DD404793F}"/>
   <bookViews>
-    <workbookView xWindow="9960" yWindow="1200" windowWidth="12984" windowHeight="6540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9960" yWindow="1200" windowWidth="12984" windowHeight="6540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Sheet" sheetId="18" r:id="rId1"/>
@@ -9955,8 +9955,8 @@
   </sheetPr>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10548,7 +10548,7 @@
   <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8A7AC5EC-FA17-4230-8D70-93F56F3DFDA8}">
           <x14:formula1>
             <xm:f>'[BMP Lego Piece (2).xlsx]Dropdownlist'!#REF!</xm:f>
@@ -10574,8 +10574,8 @@
   </sheetPr>
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
SP Update: refactor combo_bmp_maker using SQLA and Pandas
refactored code using SQLA and Pandas dataframe.
moved code to separate module: mod_Combo_BMP_Eval.py
</commit_message>
<xml_diff>
--- a/Sprint03_Data_Operation/_jonhonda_dat/special_prj/Input_Files/BMP Lego Piece.xlsx
+++ b/Sprint03_Data_Operation/_jonhonda_dat/special_prj/Input_Files/BMP Lego Piece.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Projects\Big Data School\BigDataAnalyst_ProjectDocumentation\Sprint03_Data_Operation\_jonhonda_dat\special_prj\Input_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d34c976a67baf8c/Projects/Big Data School/BigDataAnalyst_ProjectDocumentation/Sprint03_Data_Operation/_jonhonda_dat/special_prj/Input_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="86" documentId="D3CBFCB539476F3AB5D5C1344C094AEA2BA55794" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{DB4262D7-AC80-4C46-85F3-2A5DD404793F}"/>
   <bookViews>
-    <workbookView xWindow="9960" yWindow="1200" windowWidth="12984" windowHeight="6540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9960" yWindow="1200" windowWidth="12984" windowHeight="6540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary Sheet" sheetId="18" r:id="rId1"/>
@@ -1958,7 +1958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7E98C2-0016-4A4B-9FFE-BD3B62F27FF1}">
   <dimension ref="A1:AO16"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
@@ -10574,7 +10574,7 @@
   </sheetPr>
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>